<commit_message>
Corrected CTDMO reference designators, CTDMOG45 and 46 were in twice
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA03FLMA_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_GA03FLMA_00002.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="110">
   <si>
     <t>Ref Des</t>
   </si>
@@ -356,6 +356,12 @@
   </si>
   <si>
     <t>OL000031</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG046</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG047</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1223,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1252,7 +1258,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1586,10 +1592,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:Q102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="N77" sqref="N77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1605,7 +1611,7 @@
     <col min="10" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1634,7 +1640,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>50</v>
       </c>
@@ -1665,8 +1671,19 @@
       <c r="J2" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L2" s="2">
+        <f>MATCH(A2,M:M,0)</f>
+        <v>3</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" s="2">
+        <f>MATCH(M2,A:A,0)</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>50</v>
       </c>
@@ -1694,8 +1711,19 @@
       <c r="I3" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L3" s="2">
+        <f>MATCH(A3,M:M,0)</f>
+        <v>3</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>MATCH(M3,A:A,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>50</v>
       </c>
@@ -1723,8 +1751,19 @@
       <c r="I4" s="39" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L4" s="2">
+        <f>MATCH(A4,M:M,0)</f>
+        <v>3</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>MATCH(M4,A:A,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>50</v>
       </c>
@@ -1749,8 +1788,19 @@
       <c r="H5" s="39">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L5" s="2">
+        <f>MATCH(A5,M:M,0)</f>
+        <v>3</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q5" s="2">
+        <f>MATCH(M5,A:A,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>50</v>
       </c>
@@ -1775,8 +1825,19 @@
       <c r="H6" s="39">
         <v>9.06E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L6" s="2">
+        <f>MATCH(A6,M:M,0)</f>
+        <v>3</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q6" s="2">
+        <f>MATCH(M6,A:A,0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>50</v>
       </c>
@@ -1801,8 +1862,19 @@
       <c r="H7" s="39">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L7" s="2">
+        <f>MATCH(A7,M:M,0)</f>
+        <v>3</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q7" s="2">
+        <f>MATCH(M7,A:A,0)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>50</v>
       </c>
@@ -1830,8 +1902,19 @@
       <c r="I8" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L8" s="2">
+        <f>MATCH(A8,M:M,0)</f>
+        <v>3</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q8" s="2">
+        <f>MATCH(M8,A:A,0)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>50</v>
       </c>
@@ -1859,8 +1942,19 @@
       <c r="I9" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L9" s="2">
+        <f>MATCH(A9,M:M,0)</f>
+        <v>3</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q9" s="2">
+        <f>MATCH(M9,A:A,0)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>50</v>
       </c>
@@ -1888,8 +1982,19 @@
       <c r="I10" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L10" s="2">
+        <f>MATCH(A10,M:M,0)</f>
+        <v>3</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q10" s="2">
+        <f>MATCH(M10,A:A,0)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
         <v>50</v>
       </c>
@@ -1917,8 +2022,19 @@
       <c r="I11" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11" s="2">
+        <f>MATCH(A11,M:M,0)</f>
+        <v>3</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q11" s="2">
+        <f>MATCH(M11,A:A,0)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
@@ -1926,8 +2042,19 @@
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
-    </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L12" s="2" t="e">
+        <f>MATCH(A12,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q12" s="2">
+        <f>MATCH(M12,A:A,0)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>53</v>
       </c>
@@ -1958,8 +2085,19 @@
       <c r="J13" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L13" s="2">
+        <f>MATCH(A13,M:M,0)</f>
+        <v>4</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q13" s="2">
+        <f>MATCH(M13,A:A,0)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
         <v>53</v>
       </c>
@@ -1984,8 +2122,19 @@
       <c r="H14" s="31">
         <v>2229</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L14" s="2">
+        <f>MATCH(A14,M:M,0)</f>
+        <v>4</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q14" s="2">
+        <f>MATCH(M14,A:A,0)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>53</v>
       </c>
@@ -2010,8 +2159,19 @@
       <c r="H15" s="31">
         <v>101</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L15" s="2">
+        <f>MATCH(A15,M:M,0)</f>
+        <v>4</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q15" s="2">
+        <f>MATCH(M15,A:A,0)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
         <v>53</v>
       </c>
@@ -2036,8 +2196,19 @@
       <c r="H16" s="31">
         <v>38502</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L16" s="2">
+        <f>MATCH(A16,M:M,0)</f>
+        <v>4</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q16" s="2">
+        <f>MATCH(M16,A:A,0)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
         <v>53</v>
       </c>
@@ -2062,8 +2233,19 @@
       <c r="H17" s="31">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L17" s="2">
+        <f>MATCH(A17,M:M,0)</f>
+        <v>4</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q17" s="2">
+        <f>MATCH(M17,A:A,0)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>53</v>
       </c>
@@ -2088,8 +2270,19 @@
       <c r="H18" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L18" s="2">
+        <f>MATCH(A18,M:M,0)</f>
+        <v>4</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q18" s="2">
+        <f>MATCH(M18,A:A,0)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
         <v>53</v>
       </c>
@@ -2117,8 +2310,19 @@
       <c r="I19" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L19" s="2">
+        <f>MATCH(A19,M:M,0)</f>
+        <v>4</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q19" s="2">
+        <f>MATCH(M19,A:A,0)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
@@ -2126,8 +2330,12 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
-    </row>
-    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L20" s="2" t="e">
+        <f>MATCH(A20,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>47</v>
       </c>
@@ -2158,8 +2366,12 @@
       <c r="J21" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L21" s="2">
+        <f>MATCH(A21,M:M,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
         <v>47</v>
       </c>
@@ -2187,8 +2399,12 @@
       <c r="I22" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L22" s="2">
+        <f>MATCH(A22,M:M,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
         <v>47</v>
       </c>
@@ -2213,8 +2429,12 @@
       <c r="H23" s="31" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L23" s="2">
+        <f>MATCH(A23,M:M,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
@@ -2223,8 +2443,12 @@
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
       <c r="H24" s="30"/>
-    </row>
-    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L24" s="2" t="e">
+        <f>MATCH(A24,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>51</v>
       </c>
@@ -2255,8 +2479,12 @@
       <c r="J25" s="2">
         <v>500</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L25" s="2">
+        <f>MATCH(A25,M:M,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
         <v>51</v>
       </c>
@@ -2281,8 +2509,12 @@
       <c r="H26" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L26" s="2">
+        <f>MATCH(A26,M:M,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>51</v>
       </c>
@@ -2307,8 +2539,12 @@
       <c r="H27" s="32">
         <v>-42.494566666666664</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L27" s="2">
+        <f>MATCH(A27,M:M,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
         <v>51</v>
       </c>
@@ -2333,8 +2569,12 @@
       <c r="H28" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L28" s="2">
+        <f>MATCH(A28,M:M,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
         <v>51</v>
       </c>
@@ -2362,8 +2602,12 @@
       <c r="I29" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L29" s="2">
+        <f>MATCH(A29,M:M,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
         <v>51</v>
       </c>
@@ -2391,8 +2635,12 @@
       <c r="I30" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L30" s="2">
+        <f>MATCH(A30,M:M,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>51</v>
       </c>
@@ -2420,8 +2668,12 @@
       <c r="I31" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L31" s="2">
+        <f>MATCH(A31,M:M,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>51</v>
       </c>
@@ -2449,8 +2701,12 @@
       <c r="I32" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L32" s="2">
+        <f>MATCH(A32,M:M,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
         <v>51</v>
       </c>
@@ -2478,8 +2734,12 @@
       <c r="I33" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L33" s="2">
+        <f>MATCH(A33,M:M,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
@@ -2488,8 +2748,12 @@
       <c r="F34" s="29"/>
       <c r="G34" s="29"/>
       <c r="H34" s="30"/>
-    </row>
-    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L34" s="2" t="e">
+        <f>MATCH(A34,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>56</v>
       </c>
@@ -2520,8 +2784,12 @@
       <c r="J35" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L35" s="2">
+        <f>MATCH(A35,M:M,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>56</v>
       </c>
@@ -2546,8 +2814,12 @@
       <c r="H36" s="32">
         <v>-42.494566666666664</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L36" s="2">
+        <f>MATCH(A36,M:M,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>56</v>
       </c>
@@ -2572,8 +2844,12 @@
       <c r="H37" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L37" s="2">
+        <f>MATCH(A37,M:M,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
         <v>56</v>
       </c>
@@ -2598,8 +2874,12 @@
       <c r="H38" s="33">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L38" s="2">
+        <f>MATCH(A38,M:M,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
       <c r="B39" s="17"/>
       <c r="C39" s="18"/>
@@ -2608,8 +2888,12 @@
       <c r="F39" s="29"/>
       <c r="G39" s="29"/>
       <c r="H39" s="30"/>
-    </row>
-    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L39" s="2" t="e">
+        <f>MATCH(A39,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>52</v>
       </c>
@@ -2640,8 +2924,12 @@
       <c r="J40" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L40" s="2">
+        <f>MATCH(A40,M:M,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>52</v>
       </c>
@@ -2666,8 +2954,12 @@
       <c r="H41" s="32">
         <v>-42.494566666666664</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L41" s="2">
+        <f>MATCH(A41,M:M,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
         <v>52</v>
       </c>
@@ -2692,8 +2984,12 @@
       <c r="H42" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L42" s="2">
+        <f>MATCH(A42,M:M,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>52</v>
       </c>
@@ -2718,8 +3014,12 @@
       <c r="H43" s="33">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L43" s="2">
+        <f>MATCH(A43,M:M,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="17"/>
       <c r="B44" s="17"/>
       <c r="C44" s="18"/>
@@ -2728,8 +3028,12 @@
       <c r="F44" s="29"/>
       <c r="G44" s="29"/>
       <c r="H44" s="30"/>
-    </row>
-    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L44" s="2" t="e">
+        <f>MATCH(A44,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>57</v>
       </c>
@@ -2760,8 +3064,12 @@
       <c r="J45" s="2">
         <v>59</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L45" s="2">
+        <f>MATCH(A45,M:M,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
         <v>57</v>
       </c>
@@ -2786,8 +3094,12 @@
       <c r="H46" s="32">
         <v>-42.494566666666664</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L46" s="2">
+        <f>MATCH(A46,M:M,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
         <v>57</v>
       </c>
@@ -2812,8 +3124,12 @@
       <c r="H47" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L47" s="2">
+        <f>MATCH(A47,M:M,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
         <v>57</v>
       </c>
@@ -2838,8 +3154,12 @@
       <c r="H48" s="33">
         <v>42</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L48" s="2">
+        <f>MATCH(A48,M:M,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="18"/>
@@ -2848,8 +3168,12 @@
       <c r="F49" s="29"/>
       <c r="G49" s="29"/>
       <c r="H49" s="30"/>
-    </row>
-    <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L49" s="2" t="e">
+        <f>MATCH(A49,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>58</v>
       </c>
@@ -2880,8 +3204,12 @@
       <c r="J50" s="2">
         <v>90</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L50" s="2">
+        <f>MATCH(A50,M:M,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>58</v>
       </c>
@@ -2906,8 +3234,12 @@
       <c r="H51" s="32">
         <v>-42.494566666666664</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L51" s="2">
+        <f>MATCH(A51,M:M,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
         <v>58</v>
       </c>
@@ -2932,8 +3264,12 @@
       <c r="H52" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L52" s="2">
+        <f>MATCH(A52,M:M,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>58</v>
       </c>
@@ -2958,8 +3294,12 @@
       <c r="H53" s="33">
         <v>43</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L53" s="2">
+        <f>MATCH(A53,M:M,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="18"/>
@@ -2968,8 +3308,12 @@
       <c r="F54" s="29"/>
       <c r="G54" s="29"/>
       <c r="H54" s="30"/>
-    </row>
-    <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L54" s="2" t="e">
+        <f>MATCH(A54,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
         <v>59</v>
       </c>
@@ -3000,8 +3344,12 @@
       <c r="J55" s="2">
         <v>130</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L55" s="2">
+        <f>MATCH(A55,M:M,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="28" t="s">
         <v>59</v>
       </c>
@@ -3026,8 +3374,12 @@
       <c r="H56" s="32">
         <v>-42.494566666666664</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L56" s="2">
+        <f>MATCH(A56,M:M,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
         <v>59</v>
       </c>
@@ -3052,8 +3404,12 @@
       <c r="H57" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L57" s="2">
+        <f>MATCH(A57,M:M,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="28" t="s">
         <v>59</v>
       </c>
@@ -3078,8 +3434,12 @@
       <c r="H58" s="33">
         <v>44</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L58" s="2">
+        <f>MATCH(A58,M:M,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="18"/>
@@ -3088,8 +3448,12 @@
       <c r="F59" s="29"/>
       <c r="G59" s="29"/>
       <c r="H59" s="30"/>
-    </row>
-    <row r="60" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L59" s="2" t="e">
+        <f>MATCH(A59,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>60</v>
       </c>
@@ -3120,8 +3484,12 @@
       <c r="J60" s="2">
         <v>180</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L60" s="2">
+        <f>MATCH(A60,M:M,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="28" t="s">
         <v>60</v>
       </c>
@@ -3146,8 +3514,12 @@
       <c r="H61" s="32">
         <v>-42.494566666666664</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L61" s="2">
+        <f>MATCH(A61,M:M,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="28" t="s">
         <v>60</v>
       </c>
@@ -3172,8 +3544,12 @@
       <c r="H62" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L62" s="2">
+        <f>MATCH(A62,M:M,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="28" t="s">
         <v>60</v>
       </c>
@@ -3198,8 +3574,12 @@
       <c r="H63" s="33">
         <v>45</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L63" s="2">
+        <f>MATCH(A63,M:M,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="18"/>
@@ -3208,10 +3588,14 @@
       <c r="F64" s="29"/>
       <c r="G64" s="29"/>
       <c r="H64" s="30"/>
-    </row>
-    <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="17" t="s">
-        <v>59</v>
+      <c r="L64" s="2" t="e">
+        <f t="shared" ref="L64:L74" si="0">MATCH(A64,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="B65" t="s">
         <v>89</v>
@@ -3240,10 +3624,14 @@
       <c r="J65" s="2">
         <v>250</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="28" t="s">
-        <v>59</v>
+      <c r="L65" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="B66" t="s">
         <v>89</v>
@@ -3266,10 +3654,14 @@
       <c r="H66" s="32">
         <v>-42.494566666666664</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="28" t="s">
-        <v>59</v>
+      <c r="L66" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="B67" t="s">
         <v>89</v>
@@ -3292,10 +3684,14 @@
       <c r="H67" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="28" t="s">
-        <v>59</v>
+      <c r="L67" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="B68" t="s">
         <v>89</v>
@@ -3318,8 +3714,12 @@
       <c r="H68" s="33">
         <v>46</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L68" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="18"/>
@@ -3328,10 +3728,14 @@
       <c r="F69" s="29"/>
       <c r="G69" s="29"/>
       <c r="H69" s="30"/>
-    </row>
-    <row r="70" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="17" t="s">
-        <v>60</v>
+      <c r="L69" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="B70" t="s">
         <v>89</v>
@@ -3360,10 +3764,14 @@
       <c r="J70" s="2">
         <v>350</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="28" t="s">
-        <v>60</v>
+      <c r="L70" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="B71" t="s">
         <v>89</v>
@@ -3386,10 +3794,14 @@
       <c r="H71" s="32">
         <v>-42.494566666666664</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="28" t="s">
-        <v>60</v>
+      <c r="L71" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="B72" t="s">
         <v>89</v>
@@ -3412,10 +3824,14 @@
       <c r="H72" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="28" t="s">
-        <v>60</v>
+      <c r="L72" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="B73" t="s">
         <v>89</v>
@@ -3438,18 +3854,26 @@
       <c r="H73" s="33">
         <v>47</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="17"/>
-      <c r="B74" s="17"/>
+      <c r="L73" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="28"/>
+      <c r="B74"/>
       <c r="C74" s="18"/>
       <c r="D74" s="17"/>
       <c r="E74" s="17"/>
-      <c r="F74" s="29"/>
+      <c r="F74" s="36"/>
       <c r="G74" s="29"/>
-      <c r="H74" s="30"/>
-    </row>
-    <row r="75" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="H74" s="33"/>
+      <c r="L74" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="17" t="s">
         <v>61</v>
       </c>
@@ -3480,8 +3904,12 @@
       <c r="J75" s="2">
         <v>501</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L75" s="2">
+        <f>MATCH(A75,M:M,0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="28" t="s">
         <v>61</v>
       </c>
@@ -3506,8 +3934,12 @@
       <c r="H76" s="32">
         <v>-42.494566666666664</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L76" s="2">
+        <f>MATCH(A76,M:M,0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="28" t="s">
         <v>61</v>
       </c>
@@ -3532,8 +3964,12 @@
       <c r="H77" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L77" s="2">
+        <f>MATCH(A77,M:M,0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="28" t="s">
         <v>61</v>
       </c>
@@ -3558,8 +3994,12 @@
       <c r="H78" s="33">
         <v>48</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L78" s="2">
+        <f>MATCH(A78,M:M,0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="17"/>
       <c r="B79" s="17"/>
       <c r="C79" s="18"/>
@@ -3568,8 +4008,12 @@
       <c r="F79" s="19"/>
       <c r="G79" s="29"/>
       <c r="H79" s="30"/>
-    </row>
-    <row r="80" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L79" s="2" t="e">
+        <f>MATCH(A79,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
         <v>62</v>
       </c>
@@ -3600,8 +4044,12 @@
       <c r="J80" s="1">
         <v>748</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L80" s="2">
+        <f>MATCH(A80,M:M,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="28" t="s">
         <v>62</v>
       </c>
@@ -3626,8 +4074,12 @@
       <c r="H81" s="32">
         <v>-42.494566666666664</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L81" s="2">
+        <f>MATCH(A81,M:M,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="28" t="s">
         <v>62</v>
       </c>
@@ -3652,8 +4104,12 @@
       <c r="H82" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L82" s="2">
+        <f>MATCH(A82,M:M,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="28" t="s">
         <v>62</v>
       </c>
@@ -3678,8 +4134,12 @@
       <c r="H83" s="33">
         <v>49</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L83" s="2">
+        <f>MATCH(A83,M:M,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="17"/>
       <c r="B84" s="17"/>
       <c r="C84" s="18"/>
@@ -3688,8 +4148,12 @@
       <c r="F84" s="29"/>
       <c r="G84" s="29"/>
       <c r="H84" s="30"/>
-    </row>
-    <row r="85" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L84" s="2" t="e">
+        <f>MATCH(A84,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
         <v>63</v>
       </c>
@@ -3720,8 +4184,12 @@
       <c r="J85" s="2">
         <v>999</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L85" s="2">
+        <f>MATCH(A85,M:M,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="28" t="s">
         <v>63</v>
       </c>
@@ -3746,8 +4214,12 @@
       <c r="H86" s="32">
         <v>-42.494566666666664</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L86" s="2">
+        <f>MATCH(A86,M:M,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="28" t="s">
         <v>63</v>
       </c>
@@ -3772,8 +4244,12 @@
       <c r="H87" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L87" s="2">
+        <f>MATCH(A87,M:M,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="28" t="s">
         <v>63</v>
       </c>
@@ -3798,8 +4274,12 @@
       <c r="H88" s="33">
         <v>50</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L88" s="2">
+        <f>MATCH(A88,M:M,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="17"/>
       <c r="B89" s="17"/>
       <c r="C89" s="18"/>
@@ -3808,8 +4288,12 @@
       <c r="F89" s="29"/>
       <c r="G89" s="29"/>
       <c r="H89" s="30"/>
-    </row>
-    <row r="90" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L89" s="2" t="e">
+        <f>MATCH(A89,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
         <v>64</v>
       </c>
@@ -3840,8 +4324,12 @@
       <c r="J90" s="2">
         <v>1501</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L90" s="2">
+        <f>MATCH(A90,M:M,0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="28" t="s">
         <v>64</v>
       </c>
@@ -3866,8 +4354,12 @@
       <c r="H91" s="32">
         <v>-42.494566666666664</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L91" s="2">
+        <f>MATCH(A91,M:M,0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="28" t="s">
         <v>64</v>
       </c>
@@ -3892,8 +4384,12 @@
       <c r="H92" s="32">
         <v>-42.92111666666667</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L92" s="2">
+        <f>MATCH(A92,M:M,0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="28" t="s">
         <v>64</v>
       </c>
@@ -3918,8 +4414,12 @@
       <c r="H93" s="33">
         <v>51</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L93" s="2">
+        <f>MATCH(A93,M:M,0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="17"/>
       <c r="B94" s="17"/>
       <c r="C94" s="18"/>
@@ -3928,8 +4428,12 @@
       <c r="F94" s="29"/>
       <c r="G94" s="29"/>
       <c r="H94" s="30"/>
-    </row>
-    <row r="95" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L94" s="2" t="e">
+        <f>MATCH(A94,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
         <v>65</v>
       </c>
@@ -3952,8 +4456,12 @@
       <c r="H95" s="30"/>
       <c r="I95" s="30"/>
       <c r="J95" s="30"/>
-    </row>
-    <row r="96" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L95" s="2">
+        <f>MATCH(A95,M:M,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>66</v>
       </c>
@@ -3976,8 +4484,12 @@
       <c r="H96" s="30"/>
       <c r="I96" s="30"/>
       <c r="J96" s="30"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L96" s="2">
+        <f>MATCH(A96,M:M,0)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="17"/>
       <c r="B97" s="17"/>
       <c r="C97" s="18"/>
@@ -3985,8 +4497,12 @@
       <c r="E97" s="17"/>
       <c r="F97" s="17"/>
       <c r="G97" s="17"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L97" s="2" t="e">
+        <f>MATCH(A97,M:M,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="17"/>
       <c r="B98" s="17"/>
       <c r="C98" s="17"/>
@@ -3995,7 +4511,7 @@
       <c r="F98" s="17"/>
       <c r="G98" s="17"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="17"/>
       <c r="B99" s="17"/>
       <c r="C99" s="17"/>
@@ -4004,7 +4520,7 @@
       <c r="F99" s="17"/>
       <c r="G99" s="17"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
       <c r="C100" s="17"/>
@@ -4013,7 +4529,7 @@
       <c r="F100" s="17"/>
       <c r="G100" s="17"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="17"/>
       <c r="B101" s="17"/>
       <c r="C101" s="17"/>
@@ -4022,7 +4538,7 @@
       <c r="F101" s="17"/>
       <c r="G101" s="17"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="17"/>
       <c r="B102" s="17"/>
       <c r="C102" s="17"/>

</xml_diff>